<commit_message>
Probe el Process asi y jala no mover
</commit_message>
<xml_diff>
--- a/Data/Archivos_Generados/Procesados.xlsx
+++ b/Data/Archivos_Generados/Procesados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\importante\Generacion-Correo-Equipo-4\Data\Archivos_Generados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCE7998-BBF3-4133-BB21-022B861E1FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940674C7-D031-4E0F-972B-0E1D34450FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11B840C6-18A5-44F1-B45C-7D989BBECC16}"/>
   </bookViews>
@@ -33,18 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Correo Electronico</t>
-  </si>
-  <si>
-    <t>ivangarcía@beeckerco.com</t>
-  </si>
-  <si>
-    <t>allissonflores@beeckerco.com</t>
-  </si>
-  <si>
-    <t>eunice@beeckerco.com</t>
   </si>
 </sst>
 </file>
@@ -396,9 +387,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D9FC0D-26D1-4DF9-9014-3019415491E4}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -407,31 +400,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
No mover a validaciones
</commit_message>
<xml_diff>
--- a/Data/Archivos_Generados/Procesados.xlsx
+++ b/Data/Archivos_Generados/Procesados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\importante\Generacion-Correo-Equipo-4\Data\Archivos_Generados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940674C7-D031-4E0F-972B-0E1D34450FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3980C295-8844-4108-A986-603B5BE83858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11B840C6-18A5-44F1-B45C-7D989BBECC16}"/>
   </bookViews>
@@ -33,9 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Correo Electronico</t>
+  </si>
+  <si>
+    <t>IvánGarcía@beeckerco.com</t>
+  </si>
+  <si>
+    <t>AllissonFlores@beeckerco.com</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D9FC0D-26D1-4DF9-9014-3019415491E4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -400,6 +406,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>